<commit_message>
Update builtin datasets to the new COVID period format
</commit_message>
<xml_diff>
--- a/inst/shiny/WPROACM/XLSX/Japan_built_in_data.xlsx
+++ b/inst/shiny/WPROACM/XLSX/Japan_built_in_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/handcock/Build/WPROACM/inst/shiny/WPROACM/XLSX/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E316C188-E2A6-2249-99C2-23D3E2AA4096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="400" windowWidth="25600" windowHeight="14300" activeTab="1"/>
+    <workbookView xWindow="58640" yWindow="3740" windowWidth="33560" windowHeight="14300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -12,26 +18,20 @@
     <sheet name="Region1" sheetId="2" r:id="rId3"/>
     <sheet name="Region2 " sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="53">
   <si>
     <t>AGE GROUP</t>
   </si>
@@ -226,15 +226,18 @@
   <si>
     <t>100 and over</t>
   </si>
+  <si>
+    <t>START</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ###\ ##0\ ;@\ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,14 +634,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -658,6 +660,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,6 +671,18 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -676,20 +693,8 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -697,9 +702,9 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1003,15 +1008,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:A12"/>
@@ -1020,41 +1025,41 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="118.33203125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="118.33203125" style="35" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="35" customWidth="1"/>
     <col min="3" max="16384" width="8.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17" thickBot="1">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:1" ht="19" thickBot="1">
+      <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17" thickBot="1">
-      <c r="A2" s="39"/>
+    <row r="2" spans="1:1" ht="18" thickBot="1">
+      <c r="A2" s="38"/>
     </row>
-    <row r="3" spans="1:1" ht="17" thickBot="1">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:1" ht="19" thickBot="1">
+      <c r="A3" s="39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="49" thickBot="1">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:1" ht="55" thickBot="1">
+      <c r="A4" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17" thickBot="1">
-      <c r="A5" s="42"/>
+    <row r="5" spans="1:1" ht="18" thickBot="1">
+      <c r="A5" s="41"/>
     </row>
-    <row r="6" spans="1:1" ht="17" thickBot="1">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:1" ht="19" thickBot="1">
+      <c r="A6" s="42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="337" thickBot="1">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:1" ht="378" thickBot="1">
+      <c r="A7" s="43" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1084,14 +1089,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CH74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74:BV74"/>
+    <sheetView tabSelected="1" topLeftCell="BD2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="BK9" sqref="BK9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="9" customWidth="1"/>
@@ -1099,114 +1104,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="52" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="53" t="s">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="54" t="s">
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="48" t="s">
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="55"/>
+      <c r="AU1" s="55"/>
+      <c r="AV1" s="55"/>
+      <c r="AW1" s="55"/>
+      <c r="AX1" s="55"/>
+      <c r="AY1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="49" t="s">
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="BL1" s="49"/>
-      <c r="BM1" s="49"/>
-      <c r="BN1" s="49"/>
-      <c r="BO1" s="49"/>
-      <c r="BP1" s="49"/>
-      <c r="BQ1" s="49"/>
-      <c r="BR1" s="49"/>
-      <c r="BS1" s="49"/>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="49"/>
-      <c r="BV1" s="49"/>
-      <c r="BW1" s="50" t="s">
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="BX1" s="50"/>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
+      <c r="BX1" s="54"/>
+      <c r="BY1" s="54"/>
+      <c r="BZ1" s="54"/>
+      <c r="CA1" s="54"/>
+      <c r="CB1" s="54"/>
+      <c r="CC1" s="54"/>
+      <c r="CD1" s="54"/>
+      <c r="CE1" s="54"/>
+      <c r="CF1" s="54"/>
+      <c r="CG1" s="54"/>
+      <c r="CH1" s="54"/>
     </row>
     <row r="2" spans="1:86">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="34">
         <v>2015</v>
       </c>
@@ -1461,110 +1466,110 @@
       </c>
     </row>
     <row r="3" spans="1:86" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="51" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="53" t="s">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="54" t="s">
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="51"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="54"/>
-      <c r="AV3" s="54"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="54"/>
-      <c r="AY3" s="48" t="s">
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="55"/>
+      <c r="AQ3" s="55"/>
+      <c r="AR3" s="55"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="55"/>
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="55"/>
+      <c r="AW3" s="55"/>
+      <c r="AX3" s="55"/>
+      <c r="AY3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="49" t="s">
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="52"/>
+      <c r="BB3" s="52"/>
+      <c r="BC3" s="52"/>
+      <c r="BD3" s="52"/>
+      <c r="BE3" s="52"/>
+      <c r="BF3" s="52"/>
+      <c r="BG3" s="52"/>
+      <c r="BH3" s="52"/>
+      <c r="BI3" s="52"/>
+      <c r="BJ3" s="52"/>
+      <c r="BK3" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL3" s="44"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="44"/>
+      <c r="BO3" s="44"/>
+      <c r="BP3" s="44"/>
+      <c r="BQ3" s="44"/>
+      <c r="BR3" s="44"/>
+      <c r="BS3" s="44"/>
+      <c r="BT3" s="44"/>
+      <c r="BU3" s="44"/>
+      <c r="BV3" s="44"/>
+      <c r="BW3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="49"/>
-      <c r="BO3" s="49"/>
-      <c r="BP3" s="49"/>
-      <c r="BQ3" s="49"/>
-      <c r="BR3" s="49"/>
-      <c r="BS3" s="49"/>
-      <c r="BT3" s="49"/>
-      <c r="BU3" s="49"/>
-      <c r="BV3" s="49"/>
-      <c r="BW3" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="BX3" s="50"/>
-      <c r="BY3" s="50"/>
-      <c r="BZ3" s="50"/>
-      <c r="CA3" s="50"/>
-      <c r="CB3" s="50"/>
-      <c r="CC3" s="50"/>
-      <c r="CD3" s="50"/>
-      <c r="CE3" s="50"/>
-      <c r="CF3" s="50"/>
-      <c r="CG3" s="50"/>
-      <c r="CH3" s="50"/>
+      <c r="BX3" s="54"/>
+      <c r="BY3" s="54"/>
+      <c r="BZ3" s="54"/>
+      <c r="CA3" s="54"/>
+      <c r="CB3" s="54"/>
+      <c r="CC3" s="54"/>
+      <c r="CD3" s="54"/>
+      <c r="CE3" s="54"/>
+      <c r="CF3" s="54"/>
+      <c r="CG3" s="54"/>
+      <c r="CH3" s="54"/>
     </row>
     <row r="4" spans="1:86" s="9" customFormat="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -1819,8 +1824,8 @@
       </c>
     </row>
     <row r="5" spans="1:86" s="9" customFormat="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="17" t="s">
         <v>10</v>
       </c>
@@ -17295,17 +17300,15 @@
       <c r="BV74"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="O1:Z1"/>
-    <mergeCell ref="AA1:AL1"/>
-    <mergeCell ref="AY1:BJ1"/>
+  <mergeCells count="38">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="BK1:BV1"/>
     <mergeCell ref="BW1:CH1"/>
     <mergeCell ref="C3:N3"/>
@@ -17313,9 +17316,18 @@
     <mergeCell ref="AA3:AL3"/>
     <mergeCell ref="AM3:AX3"/>
     <mergeCell ref="AY3:BJ3"/>
-    <mergeCell ref="BK3:BV3"/>
     <mergeCell ref="BW3:CH3"/>
     <mergeCell ref="AM1:AX1"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AY1:BJ1"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A1:A5"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -17327,14 +17339,6 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17348,14 +17352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CH62"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="9" customWidth="1"/>
@@ -17363,114 +17367,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="52" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="53" t="s">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="54" t="s">
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="48" t="s">
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="55"/>
+      <c r="AU1" s="55"/>
+      <c r="AV1" s="55"/>
+      <c r="AW1" s="55"/>
+      <c r="AX1" s="55"/>
+      <c r="AY1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="49" t="s">
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="BL1" s="49"/>
-      <c r="BM1" s="49"/>
-      <c r="BN1" s="49"/>
-      <c r="BO1" s="49"/>
-      <c r="BP1" s="49"/>
-      <c r="BQ1" s="49"/>
-      <c r="BR1" s="49"/>
-      <c r="BS1" s="49"/>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="49"/>
-      <c r="BV1" s="49"/>
-      <c r="BW1" s="50" t="s">
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="BX1" s="50"/>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
+      <c r="BX1" s="54"/>
+      <c r="BY1" s="54"/>
+      <c r="BZ1" s="54"/>
+      <c r="CA1" s="54"/>
+      <c r="CB1" s="54"/>
+      <c r="CC1" s="54"/>
+      <c r="CD1" s="54"/>
+      <c r="CE1" s="54"/>
+      <c r="CF1" s="54"/>
+      <c r="CG1" s="54"/>
+      <c r="CH1" s="54"/>
     </row>
     <row r="2" spans="1:86">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="34">
         <v>2015</v>
       </c>
@@ -17725,110 +17729,110 @@
       </c>
     </row>
     <row r="3" spans="1:86" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="51" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="53" t="s">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="54" t="s">
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="51"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="54"/>
-      <c r="AV3" s="54"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="54"/>
-      <c r="AY3" s="48" t="s">
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="55"/>
+      <c r="AQ3" s="55"/>
+      <c r="AR3" s="55"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="55"/>
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="55"/>
+      <c r="AW3" s="55"/>
+      <c r="AX3" s="55"/>
+      <c r="AY3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="49" t="s">
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="52"/>
+      <c r="BB3" s="52"/>
+      <c r="BC3" s="52"/>
+      <c r="BD3" s="52"/>
+      <c r="BE3" s="52"/>
+      <c r="BF3" s="52"/>
+      <c r="BG3" s="52"/>
+      <c r="BH3" s="52"/>
+      <c r="BI3" s="52"/>
+      <c r="BJ3" s="52"/>
+      <c r="BK3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="49"/>
-      <c r="BO3" s="49"/>
-      <c r="BP3" s="49"/>
-      <c r="BQ3" s="49"/>
-      <c r="BR3" s="49"/>
-      <c r="BS3" s="49"/>
-      <c r="BT3" s="49"/>
-      <c r="BU3" s="49"/>
-      <c r="BV3" s="49"/>
-      <c r="BW3" s="50" t="s">
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="BX3" s="50"/>
-      <c r="BY3" s="50"/>
-      <c r="BZ3" s="50"/>
-      <c r="CA3" s="50"/>
-      <c r="CB3" s="50"/>
-      <c r="CC3" s="50"/>
-      <c r="CD3" s="50"/>
-      <c r="CE3" s="50"/>
-      <c r="CF3" s="50"/>
-      <c r="CG3" s="50"/>
-      <c r="CH3" s="50"/>
+      <c r="BX3" s="54"/>
+      <c r="BY3" s="54"/>
+      <c r="BZ3" s="54"/>
+      <c r="CA3" s="54"/>
+      <c r="CB3" s="54"/>
+      <c r="CC3" s="54"/>
+      <c r="CD3" s="54"/>
+      <c r="CE3" s="54"/>
+      <c r="CF3" s="54"/>
+      <c r="CG3" s="54"/>
+      <c r="CH3" s="54"/>
     </row>
     <row r="4" spans="1:86" s="9" customFormat="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -18083,8 +18087,8 @@
       </c>
     </row>
     <row r="5" spans="1:86" s="9" customFormat="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="17" t="s">
         <v>10</v>
       </c>
@@ -18338,7 +18342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="15">
+    <row r="6" spans="1:86">
       <c r="A6" s="45" t="s">
         <v>22</v>
       </c>
@@ -18430,7 +18434,7 @@
       <c r="CG6" s="33"/>
       <c r="CH6" s="33"/>
     </row>
-    <row r="7" spans="1:86" ht="15">
+    <row r="7" spans="1:86">
       <c r="A7" s="46"/>
       <c r="B7" s="31" t="s">
         <v>23</v>
@@ -18520,7 +18524,7 @@
       <c r="CG7" s="33"/>
       <c r="CH7" s="33"/>
     </row>
-    <row r="8" spans="1:86" ht="15">
+    <row r="8" spans="1:86">
       <c r="A8" s="47"/>
       <c r="B8" s="31" t="s">
         <v>24</v>
@@ -18610,7 +18614,7 @@
       <c r="CG8" s="33"/>
       <c r="CH8" s="33"/>
     </row>
-    <row r="9" spans="1:86" ht="15">
+    <row r="9" spans="1:86">
       <c r="A9" s="45"/>
       <c r="B9" s="31" t="s">
         <v>22</v>
@@ -18700,7 +18704,7 @@
       <c r="CG9" s="33"/>
       <c r="CH9" s="33"/>
     </row>
-    <row r="10" spans="1:86" ht="15">
+    <row r="10" spans="1:86">
       <c r="A10" s="46"/>
       <c r="B10" s="31" t="s">
         <v>23</v>
@@ -18790,7 +18794,7 @@
       <c r="CG10" s="33"/>
       <c r="CH10" s="33"/>
     </row>
-    <row r="11" spans="1:86" ht="15">
+    <row r="11" spans="1:86">
       <c r="A11" s="47"/>
       <c r="B11" s="31" t="s">
         <v>24</v>
@@ -18880,7 +18884,7 @@
       <c r="CG11" s="33"/>
       <c r="CH11" s="33"/>
     </row>
-    <row r="12" spans="1:86" ht="15">
+    <row r="12" spans="1:86">
       <c r="A12" s="45"/>
       <c r="B12" s="31" t="s">
         <v>22</v>
@@ -18970,7 +18974,7 @@
       <c r="CG12" s="33"/>
       <c r="CH12" s="33"/>
     </row>
-    <row r="13" spans="1:86" ht="15">
+    <row r="13" spans="1:86">
       <c r="A13" s="46"/>
       <c r="B13" s="31" t="s">
         <v>23</v>
@@ -19060,7 +19064,7 @@
       <c r="CG13" s="33"/>
       <c r="CH13" s="33"/>
     </row>
-    <row r="14" spans="1:86" ht="15">
+    <row r="14" spans="1:86">
       <c r="A14" s="47"/>
       <c r="B14" s="31" t="s">
         <v>24</v>
@@ -19150,7 +19154,7 @@
       <c r="CG14" s="33"/>
       <c r="CH14" s="33"/>
     </row>
-    <row r="15" spans="1:86" ht="15">
+    <row r="15" spans="1:86">
       <c r="A15" s="45"/>
       <c r="B15" s="31" t="s">
         <v>22</v>
@@ -19240,7 +19244,7 @@
       <c r="CG15" s="33"/>
       <c r="CH15" s="33"/>
     </row>
-    <row r="16" spans="1:86" ht="15">
+    <row r="16" spans="1:86">
       <c r="A16" s="46"/>
       <c r="B16" s="31" t="s">
         <v>23</v>
@@ -19330,7 +19334,7 @@
       <c r="CG16" s="33"/>
       <c r="CH16" s="33"/>
     </row>
-    <row r="17" spans="1:86" ht="15">
+    <row r="17" spans="1:86">
       <c r="A17" s="47"/>
       <c r="B17" s="31" t="s">
         <v>24</v>
@@ -23472,13 +23476,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AY1:BJ1"/>
+    <mergeCell ref="BK1:BV1"/>
+    <mergeCell ref="BW1:CH1"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="AA3:AL3"/>
+    <mergeCell ref="AM3:AX3"/>
+    <mergeCell ref="AY3:BJ3"/>
+    <mergeCell ref="BK3:BV3"/>
+    <mergeCell ref="BW3:CH3"/>
+    <mergeCell ref="AM1:AX1"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -23491,22 +23504,13 @@
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="AY1:BJ1"/>
-    <mergeCell ref="BK1:BV1"/>
-    <mergeCell ref="BW1:CH1"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="O3:Z3"/>
-    <mergeCell ref="AA3:AL3"/>
-    <mergeCell ref="AM3:AX3"/>
-    <mergeCell ref="AY3:BJ3"/>
-    <mergeCell ref="BK3:BV3"/>
-    <mergeCell ref="BW3:CH3"/>
-    <mergeCell ref="AM1:AX1"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="O1:Z1"/>
-    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -23521,14 +23525,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CH62"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="9" customWidth="1"/>
@@ -23536,114 +23540,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="52" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="53" t="s">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="54" t="s">
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="48" t="s">
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="55"/>
+      <c r="AU1" s="55"/>
+      <c r="AV1" s="55"/>
+      <c r="AW1" s="55"/>
+      <c r="AX1" s="55"/>
+      <c r="AY1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="49" t="s">
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="BL1" s="49"/>
-      <c r="BM1" s="49"/>
-      <c r="BN1" s="49"/>
-      <c r="BO1" s="49"/>
-      <c r="BP1" s="49"/>
-      <c r="BQ1" s="49"/>
-      <c r="BR1" s="49"/>
-      <c r="BS1" s="49"/>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="49"/>
-      <c r="BV1" s="49"/>
-      <c r="BW1" s="50" t="s">
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="BX1" s="50"/>
-      <c r="BY1" s="50"/>
-      <c r="BZ1" s="50"/>
-      <c r="CA1" s="50"/>
-      <c r="CB1" s="50"/>
-      <c r="CC1" s="50"/>
-      <c r="CD1" s="50"/>
-      <c r="CE1" s="50"/>
-      <c r="CF1" s="50"/>
-      <c r="CG1" s="50"/>
-      <c r="CH1" s="50"/>
+      <c r="BX1" s="54"/>
+      <c r="BY1" s="54"/>
+      <c r="BZ1" s="54"/>
+      <c r="CA1" s="54"/>
+      <c r="CB1" s="54"/>
+      <c r="CC1" s="54"/>
+      <c r="CD1" s="54"/>
+      <c r="CE1" s="54"/>
+      <c r="CF1" s="54"/>
+      <c r="CG1" s="54"/>
+      <c r="CH1" s="54"/>
     </row>
     <row r="2" spans="1:86">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="34">
         <v>2015</v>
       </c>
@@ -23898,110 +23902,110 @@
       </c>
     </row>
     <row r="3" spans="1:86" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="51" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="53" t="s">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="54" t="s">
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="51"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="54"/>
-      <c r="AV3" s="54"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="54"/>
-      <c r="AY3" s="48" t="s">
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="55"/>
+      <c r="AQ3" s="55"/>
+      <c r="AR3" s="55"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="55"/>
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="55"/>
+      <c r="AW3" s="55"/>
+      <c r="AX3" s="55"/>
+      <c r="AY3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="49" t="s">
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="52"/>
+      <c r="BB3" s="52"/>
+      <c r="BC3" s="52"/>
+      <c r="BD3" s="52"/>
+      <c r="BE3" s="52"/>
+      <c r="BF3" s="52"/>
+      <c r="BG3" s="52"/>
+      <c r="BH3" s="52"/>
+      <c r="BI3" s="52"/>
+      <c r="BJ3" s="52"/>
+      <c r="BK3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="49"/>
-      <c r="BO3" s="49"/>
-      <c r="BP3" s="49"/>
-      <c r="BQ3" s="49"/>
-      <c r="BR3" s="49"/>
-      <c r="BS3" s="49"/>
-      <c r="BT3" s="49"/>
-      <c r="BU3" s="49"/>
-      <c r="BV3" s="49"/>
-      <c r="BW3" s="50" t="s">
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="BX3" s="50"/>
-      <c r="BY3" s="50"/>
-      <c r="BZ3" s="50"/>
-      <c r="CA3" s="50"/>
-      <c r="CB3" s="50"/>
-      <c r="CC3" s="50"/>
-      <c r="CD3" s="50"/>
-      <c r="CE3" s="50"/>
-      <c r="CF3" s="50"/>
-      <c r="CG3" s="50"/>
-      <c r="CH3" s="50"/>
+      <c r="BX3" s="54"/>
+      <c r="BY3" s="54"/>
+      <c r="BZ3" s="54"/>
+      <c r="CA3" s="54"/>
+      <c r="CB3" s="54"/>
+      <c r="CC3" s="54"/>
+      <c r="CD3" s="54"/>
+      <c r="CE3" s="54"/>
+      <c r="CF3" s="54"/>
+      <c r="CG3" s="54"/>
+      <c r="CH3" s="54"/>
     </row>
     <row r="4" spans="1:86" s="9" customFormat="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -24256,8 +24260,8 @@
       </c>
     </row>
     <row r="5" spans="1:86" s="9" customFormat="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="17" t="s">
         <v>10</v>
       </c>
@@ -24511,7 +24515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="15">
+    <row r="6" spans="1:86">
       <c r="A6" s="45" t="s">
         <v>22</v>
       </c>
@@ -24603,7 +24607,7 @@
       <c r="CG6" s="33"/>
       <c r="CH6" s="33"/>
     </row>
-    <row r="7" spans="1:86" ht="15">
+    <row r="7" spans="1:86">
       <c r="A7" s="46"/>
       <c r="B7" s="31" t="s">
         <v>23</v>
@@ -24693,7 +24697,7 @@
       <c r="CG7" s="33"/>
       <c r="CH7" s="33"/>
     </row>
-    <row r="8" spans="1:86" ht="15">
+    <row r="8" spans="1:86">
       <c r="A8" s="47"/>
       <c r="B8" s="31" t="s">
         <v>24</v>
@@ -24783,7 +24787,7 @@
       <c r="CG8" s="33"/>
       <c r="CH8" s="33"/>
     </row>
-    <row r="9" spans="1:86" ht="15">
+    <row r="9" spans="1:86">
       <c r="A9" s="45"/>
       <c r="B9" s="31" t="s">
         <v>22</v>
@@ -24873,7 +24877,7 @@
       <c r="CG9" s="33"/>
       <c r="CH9" s="33"/>
     </row>
-    <row r="10" spans="1:86" ht="15">
+    <row r="10" spans="1:86">
       <c r="A10" s="46"/>
       <c r="B10" s="31" t="s">
         <v>23</v>
@@ -24963,7 +24967,7 @@
       <c r="CG10" s="33"/>
       <c r="CH10" s="33"/>
     </row>
-    <row r="11" spans="1:86" ht="15">
+    <row r="11" spans="1:86">
       <c r="A11" s="47"/>
       <c r="B11" s="31" t="s">
         <v>24</v>
@@ -25053,7 +25057,7 @@
       <c r="CG11" s="33"/>
       <c r="CH11" s="33"/>
     </row>
-    <row r="12" spans="1:86" ht="15">
+    <row r="12" spans="1:86">
       <c r="A12" s="45"/>
       <c r="B12" s="31" t="s">
         <v>22</v>
@@ -25143,7 +25147,7 @@
       <c r="CG12" s="33"/>
       <c r="CH12" s="33"/>
     </row>
-    <row r="13" spans="1:86" ht="15">
+    <row r="13" spans="1:86">
       <c r="A13" s="46"/>
       <c r="B13" s="31" t="s">
         <v>23</v>
@@ -25233,7 +25237,7 @@
       <c r="CG13" s="33"/>
       <c r="CH13" s="33"/>
     </row>
-    <row r="14" spans="1:86" ht="15">
+    <row r="14" spans="1:86">
       <c r="A14" s="47"/>
       <c r="B14" s="31" t="s">
         <v>24</v>
@@ -25323,7 +25327,7 @@
       <c r="CG14" s="33"/>
       <c r="CH14" s="33"/>
     </row>
-    <row r="15" spans="1:86" ht="15">
+    <row r="15" spans="1:86">
       <c r="A15" s="45"/>
       <c r="B15" s="31" t="s">
         <v>22</v>
@@ -25413,7 +25417,7 @@
       <c r="CG15" s="33"/>
       <c r="CH15" s="33"/>
     </row>
-    <row r="16" spans="1:86" ht="15">
+    <row r="16" spans="1:86">
       <c r="A16" s="46"/>
       <c r="B16" s="31" t="s">
         <v>23</v>
@@ -25503,7 +25507,7 @@
       <c r="CG16" s="33"/>
       <c r="CH16" s="33"/>
     </row>
-    <row r="17" spans="1:86" ht="15">
+    <row r="17" spans="1:86">
       <c r="A17" s="47"/>
       <c r="B17" s="31" t="s">
         <v>24</v>
@@ -29645,13 +29649,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="AY1:BJ1"/>
+    <mergeCell ref="BK1:BV1"/>
+    <mergeCell ref="BW1:CH1"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="AA3:AL3"/>
+    <mergeCell ref="AM3:AX3"/>
+    <mergeCell ref="AY3:BJ3"/>
+    <mergeCell ref="BK3:BV3"/>
+    <mergeCell ref="BW3:CH3"/>
+    <mergeCell ref="AM1:AX1"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -29664,22 +29677,13 @@
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="AY1:BJ1"/>
-    <mergeCell ref="BK1:BV1"/>
-    <mergeCell ref="BW1:CH1"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="O3:Z3"/>
-    <mergeCell ref="AA3:AL3"/>
-    <mergeCell ref="AM3:AX3"/>
-    <mergeCell ref="AY3:BJ3"/>
-    <mergeCell ref="BK3:BV3"/>
-    <mergeCell ref="BW3:CH3"/>
-    <mergeCell ref="AM1:AX1"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="O1:Z1"/>
-    <mergeCell ref="AA1:AL1"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>